<commit_message>
editing errors, updating graphs
</commit_message>
<xml_diff>
--- a/Dow 30/Apple/Apple DCF.xlsx
+++ b/Dow 30/Apple/Apple DCF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shashwat Sharma\Documents\DCF\Dow 30\Apple\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E878386-FB85-4BE5-9A99-356763A358B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B168DA-3833-4D57-84F3-58181199AD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{08B3BD42-F7E2-4899-946D-496009338604}"/>
+    <workbookView xWindow="23880" yWindow="-7830" windowWidth="24240" windowHeight="18240" activeTab="1" xr2:uid="{08B3BD42-F7E2-4899-946D-496009338604}"/>
   </bookViews>
   <sheets>
     <sheet name="Street Estimates" sheetId="1" r:id="rId1"/>
@@ -766,7 +766,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,9 +940,7 @@
       <c r="L8" s="41">
         <v>125700</v>
       </c>
-      <c r="M8" s="41">
-        <v>124000</v>
-      </c>
+      <c r="M8" s="41"/>
       <c r="N8" s="41">
         <v>141000</v>
       </c>
@@ -1012,7 +1010,7 @@
       </c>
       <c r="M10" s="8">
         <f t="shared" si="0"/>
-        <v>22320</v>
+        <v>0</v>
       </c>
       <c r="N10" s="8">
         <f t="shared" si="0"/>
@@ -1207,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B2B475-E092-48FC-990D-00D6632DE395}">
   <dimension ref="B2:O46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -1294,7 +1292,7 @@
       </c>
       <c r="N6" s="37">
         <f>'Street Estimates'!M8</f>
-        <v>124000</v>
+        <v>0</v>
       </c>
       <c r="O6" s="37">
         <f>'Street Estimates'!N8</f>
@@ -1331,7 +1329,7 @@
       </c>
       <c r="N7" s="10">
         <f>-'Street Estimates'!M10</f>
-        <v>-22320</v>
+        <v>0</v>
       </c>
       <c r="O7" s="10">
         <f>-'Street Estimates'!N10</f>
@@ -1487,7 +1485,7 @@
       </c>
       <c r="N11" s="10">
         <f t="shared" si="0"/>
-        <v>132876</v>
+        <v>31196</v>
       </c>
       <c r="O11" s="10">
         <f t="shared" si="0"/>
@@ -1716,24 +1714,24 @@
         <v>41</v>
       </c>
       <c r="G33" s="10">
-        <f>J11*G32</f>
-        <v>126025.09755697903</v>
+        <f>K11*G32</f>
+        <v>127587.1312910563</v>
       </c>
       <c r="H33" s="10">
-        <f t="shared" ref="H33:K33" si="1">K11*H32</f>
-        <v>122968.71914035641</v>
+        <f t="shared" ref="H33:K33" si="1">L11*H32</f>
+        <v>122073.24595162328</v>
       </c>
       <c r="I33" s="10">
         <f t="shared" si="1"/>
-        <v>117654.42599169933</v>
+        <v>118279.33783085168</v>
       </c>
       <c r="J33" s="10">
         <f t="shared" si="1"/>
-        <v>113997.85014877039</v>
+        <v>26918.448095501892</v>
       </c>
       <c r="K33" s="10">
         <f t="shared" si="1"/>
-        <v>110505.89065343038</v>
+        <v>115993.09576595134</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
@@ -1754,7 +1752,7 @@
       <c r="E35" s="31"/>
       <c r="F35" s="30">
         <f>SUM(G33:K34)</f>
-        <v>4128058.6145626525</v>
+        <v>4047757.8900064016</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -1806,7 +1804,7 @@
       <c r="C42" s="48"/>
       <c r="F42" s="29">
         <f>F35+F38-F40-F41</f>
-        <v>4075598.6145626525</v>
+        <v>3995297.8900064016</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -1826,7 +1824,7 @@
       </c>
       <c r="F45" s="25">
         <f>F42/F44</f>
-        <v>246.55768993119494</v>
+        <v>241.69981185761654</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -1835,7 +1833,7 @@
       </c>
       <c r="F46" s="25">
         <f>F45-147.02</f>
-        <v>99.537689931194933</v>
+        <v>94.679811857616528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new value for apple, added historical "estimates"
</commit_message>
<xml_diff>
--- a/Dow 30/Apple/Apple DCF.xlsx
+++ b/Dow 30/Apple/Apple DCF.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shashwat Sharma\Documents\DCF\Dow 30\Apple\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shashwat Sharma\Documents\Dow Valuation\Dow 30\Apple\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA22BD8-372D-47E2-9B59-9519B887E1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B4DA7B-B41E-4E00-BC57-C37196972834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{08B3BD42-F7E2-4899-946D-496009338604}"/>
+    <workbookView xWindow="23880" yWindow="-6750" windowWidth="24240" windowHeight="18240" activeTab="3" xr2:uid="{08B3BD42-F7E2-4899-946D-496009338604}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical Data" sheetId="3" r:id="rId1"/>
     <sheet name="Street Estimates" sheetId="1" r:id="rId2"/>
     <sheet name="DCF Model" sheetId="2" r:id="rId3"/>
+    <sheet name="Historical Estimates" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>Ticker: AAPL</t>
   </si>
@@ -241,6 +242,18 @@
   </si>
   <si>
     <t>EBT, Unusual Items</t>
+  </si>
+  <si>
+    <t>Current Price</t>
+  </si>
+  <si>
+    <t>CAGR</t>
+  </si>
+  <si>
+    <t>Intrinsic Value</t>
+  </si>
+  <si>
+    <t>(5-year estimates)</t>
   </si>
 </sst>
 </file>
@@ -445,7 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -532,6 +545,9 @@
     <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2511,8 +2527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B2B475-E092-48FC-990D-00D6632DE395}">
   <dimension ref="B2:O46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3149,4 +3165,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA492CD5-AB56-4D55-B27E-4CE775C80393}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="78">
+        <v>44765</v>
+      </c>
+      <c r="B2">
+        <v>154.09</v>
+      </c>
+      <c r="C2" s="80">
+        <v>241.7</v>
+      </c>
+      <c r="D2">
+        <v>87.61</v>
+      </c>
+      <c r="E2" s="79">
+        <v>9.4200000000000006E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="78">
+        <v>44774</v>
+      </c>
+      <c r="B3">
+        <v>161.51</v>
+      </c>
+      <c r="C3">
+        <v>179.49</v>
+      </c>
+      <c r="D3">
+        <v>17.98</v>
+      </c>
+      <c r="E3" s="79">
+        <v>2.1299999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>